<commit_message>
ran final tests and updated spreadsheet
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Graph</t>
   </si>
@@ -35,12 +35,6 @@
     <t>Edges</t>
   </si>
   <si>
-    <t>Avg. In degree</t>
-  </si>
-  <si>
-    <t>Avg. Out Degree</t>
-  </si>
-  <si>
     <t>Avg. Clustering Coeff</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>FRDG</t>
   </si>
   <si>
-    <t>FRDG-TCL</t>
-  </si>
-  <si>
     <t>RW-25</t>
   </si>
   <si>
@@ -102,14 +93,175 @@
   </si>
   <si>
     <t>FRDG-Rand-50</t>
+  </si>
+  <si>
+    <t>FRDG-TCL-P</t>
+  </si>
+  <si>
+    <t>FRDG-TCL-.6</t>
+  </si>
+  <si>
+    <t>Reciprocal Edges</t>
+  </si>
+  <si>
+    <t>FRDG-Rand-25</t>
+  </si>
+  <si>
+    <t>Underestimates low degrees, but conveges to original at higher degrees</t>
+  </si>
+  <si>
+    <t>Overests low degrees, but underestimates by a nearly fixed amount in higher degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimates low degrees, but converges to fixed underestimate - LOWEST </t>
+  </si>
+  <si>
+    <t>Underests low degrees, but converges to random 50's distro in higher degrees</t>
+  </si>
+  <si>
+    <t>Blowup factor leads to overest of degree 0, but underests other low degrees. Converges to original</t>
+  </si>
+  <si>
+    <t>Overests low degrees, then slightly underestimates high degrees</t>
+  </si>
+  <si>
+    <t>Blowup ruins low degrees worst here, then converges to fixed underest of original</t>
+  </si>
+  <si>
+    <t>Same blowup effect, but converges to rand 50's distro</t>
+  </si>
+  <si>
+    <t>Completely flat</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Mimics shape of distro, but underestimates until very large degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimates well in low hops, but overests in high hops </t>
+  </si>
+  <si>
+    <t>Fixed underestimate</t>
+  </si>
+  <si>
+    <t>biggest fixed underestimate</t>
+  </si>
+  <si>
+    <t>Follows random 50, then converges to original</t>
+  </si>
+  <si>
+    <t>0 degree is accurate, but low degrees underest. Converges to original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">underests low degrees, then converges to fixed underestimate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">underests low degrees, and converges to 50% sample </t>
+  </si>
+  <si>
+    <t>follows frdg-rand-50 then underests the biggest</t>
+  </si>
+  <si>
+    <t>Overestimates across all hops</t>
+  </si>
+  <si>
+    <t>overests in &gt;2 hops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slightly overests in &gt;4 hops </t>
+  </si>
+  <si>
+    <t>huge underest</t>
+  </si>
+  <si>
+    <t>huge underest and short distro</t>
+  </si>
+  <si>
+    <t>underests, then overests, then converges to original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">underests 0 degree, then overests </t>
+  </si>
+  <si>
+    <t>huge underest of low degrees then converges to overest of high degrees</t>
+  </si>
+  <si>
+    <t>slightly over TCL in low degrees, but closer overest at high degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">follows above </t>
+  </si>
+  <si>
+    <t xml:space="preserve">follows shape of original, but decreases to 0 </t>
+  </si>
+  <si>
+    <t>huge underestimate, but does not follow shape of original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">underests 50% version by a fixed amount </t>
+  </si>
+  <si>
+    <t>huge underest, does not mimic shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overests low degrees more than 50%, then underests more than 50% </t>
+  </si>
+  <si>
+    <t>slightly underests rand-50</t>
+  </si>
+  <si>
+    <t>bigger fixed underest than rand-50</t>
+  </si>
+  <si>
+    <t>huger underest, does not mimic shape</t>
+  </si>
+  <si>
+    <t>smaller version of rand-50</t>
+  </si>
+  <si>
+    <t>Avg. degree</t>
+  </si>
+  <si>
+    <t>Node err</t>
+  </si>
+  <si>
+    <t>Edge Err</t>
+  </si>
+  <si>
+    <t>Avg. Degree Err</t>
+  </si>
+  <si>
+    <t>ACC err.</t>
+  </si>
+  <si>
+    <t>Recip Edge Err</t>
+  </si>
+  <si>
+    <t>reciprocity err</t>
+  </si>
+  <si>
+    <t>LSCC edge err</t>
+  </si>
+  <si>
+    <t>LSCC node err</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,8 +289,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,130 +575,1024 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" customWidth="1"/>
-    <col min="13" max="13" width="24.88671875" customWidth="1"/>
-    <col min="14" max="14" width="16.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="19.44140625" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
+    <col min="10" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="15" width="16.109375" customWidth="1"/>
+    <col min="16" max="17" width="16.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
+    <col min="19" max="19" width="22.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.88671875" customWidth="1"/>
+    <col min="21" max="21" width="24.88671875" customWidth="1"/>
+    <col min="22" max="22" width="21.77734375" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" customWidth="1"/>
+    <col min="24" max="24" width="24.44140625" customWidth="1"/>
+    <col min="25" max="25" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="S1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="T1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="U1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="V1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="W1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="X1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B2">
+        <v>81306</v>
+      </c>
+      <c r="D2">
+        <v>1768149</v>
+      </c>
+      <c r="F2">
+        <v>43.5</v>
+      </c>
+      <c r="H2">
+        <v>0.56531100000000001</v>
+      </c>
+      <c r="J2">
+        <v>851692</v>
+      </c>
+      <c r="L2">
+        <f>J2/D2</f>
+        <v>0.48168564979535095</v>
+      </c>
+      <c r="N2">
+        <v>68413</v>
+      </c>
+      <c r="P2">
+        <v>1685163</v>
+      </c>
+      <c r="R2">
+        <v>14</v>
+      </c>
+      <c r="S2">
+        <v>15</v>
+      </c>
+      <c r="T2">
+        <v>14</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B3">
+        <v>78665</v>
+      </c>
+      <c r="C3">
+        <f>1- B3/$B$2</f>
+        <v>3.2482227633876981E-2</v>
+      </c>
+      <c r="D3">
+        <v>2352970</v>
+      </c>
+      <c r="E3">
+        <f>1-(D2/D3)</f>
+        <v>0.24854588031296621</v>
+      </c>
+      <c r="F3">
+        <v>60.1</v>
+      </c>
+      <c r="G3">
+        <f>1-(F2/F3)</f>
+        <v>0.27620632279534107</v>
+      </c>
+      <c r="H3">
+        <v>5.7831E-2</v>
+      </c>
+      <c r="I3">
+        <f>1-(H3/H$2)</f>
+        <v>0.89770055774609014</v>
+      </c>
+      <c r="J3">
+        <v>58598</v>
+      </c>
+      <c r="K3">
+        <f>1-(J3/J$2)</f>
+        <v>0.93119813265828488</v>
+      </c>
+      <c r="L3">
+        <f>J3/D3</f>
+        <v>2.4903844927899633E-2</v>
+      </c>
+      <c r="M3">
+        <f>1-(L3/L$2)</f>
+        <v>0.94829855334390745</v>
+      </c>
+      <c r="N3">
+        <v>64293</v>
+      </c>
+      <c r="O3">
+        <f>1-(N3/N$2)</f>
+        <v>6.0222472337128963E-2</v>
+      </c>
+      <c r="P3">
+        <v>2271300</v>
+      </c>
+      <c r="Q3">
+        <f>1-(P2/P3)</f>
+        <v>0.25806234315149912</v>
+      </c>
+      <c r="R3">
+        <v>8</v>
+      </c>
+      <c r="S3">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:25" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B4">
+        <v>80776</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="0">1- B4/$B$2</f>
+        <v>6.5185841143334811E-3</v>
+      </c>
+      <c r="D4">
+        <v>1730617</v>
+      </c>
+      <c r="E4">
+        <f>1-(D4/$D$2)</f>
+        <v>2.1226717884069712E-2</v>
+      </c>
+      <c r="F4">
+        <v>42.8</v>
+      </c>
+      <c r="G4">
+        <f>1-(F4/$F$2)</f>
+        <v>1.6091954022988575E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.496E-3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:K14" si="1">1-(H4/H$2)</f>
+        <v>0.99204685562460304</v>
+      </c>
+      <c r="J4">
+        <v>819694</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>3.7569919642312044E-2</v>
+      </c>
+      <c r="L4">
+        <f>J4/D4</f>
+        <v>0.47364263727907446</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4" si="2">1-(L4/L$2)</f>
+        <v>1.6697637805265009E-2</v>
+      </c>
+      <c r="N4">
+        <v>67803</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4" si="3">1-(N4/N$2)</f>
+        <v>8.9164340110797768E-3</v>
+      </c>
+      <c r="P4">
+        <v>1577568</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4" si="4">1-(P4/P$2)</f>
+        <v>6.3848422971546359E-2</v>
+      </c>
+      <c r="R4">
+        <v>14</v>
+      </c>
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="T4">
+        <v>14</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>79090</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2.7255061127100078E-2</v>
+      </c>
+      <c r="D5">
+        <v>1699181</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E14" si="5">1-(D5/$D$2)</f>
+        <v>3.9005762523407261E-2</v>
+      </c>
+      <c r="F5">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G14" si="6">1-(F5/$F$2)</f>
+        <v>1.1494252873563204E-2</v>
+      </c>
+      <c r="H5">
+        <v>6.0039000000000002E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.89379474307062834</v>
+      </c>
+      <c r="J5">
+        <v>18550</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.97821982594646895</v>
+      </c>
+      <c r="L5">
+        <f>J5/D5</f>
+        <v>1.0917024142807622E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5" si="7">1-(L5/L$2)</f>
+        <v>0.97733579120024472</v>
+      </c>
+      <c r="N5">
+        <v>62450</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5" si="8">1-(N5/N$2)</f>
+        <v>8.7161796734538721E-2</v>
+      </c>
+      <c r="P5">
+        <v>1547578</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5" si="9">1-(P5/P$2)</f>
+        <v>8.164492099577314E-2</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5">
+        <v>9</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>78786</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3.0994022581359304E-2</v>
+      </c>
+      <c r="D6">
+        <v>1634509</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="5"/>
+        <v>7.5581865555448102E-2</v>
+      </c>
+      <c r="F6">
+        <v>41.5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="6"/>
+        <v>4.5977011494252928E-2</v>
+      </c>
+      <c r="H6">
+        <v>5.8770000000000003E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0.89603952514633534</v>
+      </c>
+      <c r="J6">
+        <v>5557</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>0.99347534085091793</v>
+      </c>
+      <c r="L6">
+        <f>J6/D6</f>
+        <v>3.3997977374245108E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6" si="10">1-(L6/L$2)</f>
+        <v>0.99294187456307048</v>
+      </c>
+      <c r="N6">
+        <v>57402</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="11">1-(N6/N$2)</f>
+        <v>0.16094894245245783</v>
+      </c>
+      <c r="P6">
+        <v>1275092</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6" si="12">1-(P6/P$2)</f>
+        <v>0.24334203872266358</v>
+      </c>
+      <c r="R6">
+        <v>14</v>
+      </c>
+      <c r="S6">
+        <v>14</v>
+      </c>
+      <c r="T6">
+        <v>13</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B8">
+        <v>14845</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.81741814872211149</v>
+      </c>
+      <c r="D8">
+        <v>115974</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="5"/>
+        <v>0.93440937387064094</v>
+      </c>
+      <c r="F8">
+        <v>15.6</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="6"/>
+        <v>0.64137931034482754</v>
+      </c>
+      <c r="H8">
+        <v>0.211508</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.625855502546386</v>
+      </c>
+      <c r="J8">
+        <v>42046</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.95063238823424434</v>
+      </c>
+      <c r="L8">
+        <f>J8/D8</f>
+        <v>0.36254677772604205</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8" si="13">1-(L8/L$2)</f>
+        <v>0.24733739134625721</v>
+      </c>
+      <c r="N8">
+        <v>11865</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8" si="14">1-(N8/N$2)</f>
+        <v>0.82656804993203048</v>
+      </c>
+      <c r="P8">
+        <v>110599</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8" si="15">1-(P8/P$2)</f>
+        <v>0.93436896015400295</v>
+      </c>
+      <c r="R8">
+        <v>31</v>
+      </c>
+      <c r="S8">
+        <v>31</v>
+      </c>
+      <c r="T8">
+        <v>29</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B9">
+        <v>26795</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.67044252576685603</v>
+      </c>
+      <c r="D9">
+        <v>144092</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="5"/>
+        <v>0.91850686791667446</v>
+      </c>
+      <c r="F9">
+        <v>11.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>0.73563218390804597</v>
+      </c>
+      <c r="H9">
+        <v>0.19487299999999999</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.65528178294779338</v>
+      </c>
+      <c r="J9">
+        <v>40520</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.9524241157601574</v>
+      </c>
+      <c r="L9">
+        <f>J9/D9</f>
+        <v>0.28120922743802573</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9" si="16">1-(L9/L$2)</f>
+        <v>0.41619762274940031</v>
+      </c>
+      <c r="N9">
+        <v>22230</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="17">1-(N9/N$2)</f>
+        <v>0.67506175726835549</v>
+      </c>
+      <c r="P9">
+        <v>144092</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9" si="18">1-(P9/P$2)</f>
+        <v>0.91449373146692636</v>
+      </c>
+      <c r="R9">
+        <v>27</v>
+      </c>
+      <c r="S9">
+        <v>28</v>
+      </c>
+      <c r="T9">
+        <v>26</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="10" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B10">
+        <v>70931</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.12760435884190591</v>
+      </c>
+      <c r="D10">
+        <v>531032</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>0.69966784473480459</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="6"/>
+        <v>0.65517241379310343</v>
+      </c>
+      <c r="H10">
+        <v>0.207813</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.63239172773924435</v>
+      </c>
+      <c r="J10">
+        <v>102012</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.88022430643941707</v>
+      </c>
+      <c r="L10">
+        <f>J10/D10</f>
+        <v>0.19210141761701743</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="19">1-(L10/L$2)</f>
+        <v>0.60118924510490679</v>
+      </c>
+      <c r="N10">
+        <v>44837</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ref="O10" si="20">1-(N10/N$2)</f>
+        <v>0.34461286597576479</v>
+      </c>
+      <c r="P10">
+        <v>458076</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10" si="21">1-(P10/P$2)</f>
+        <v>0.72817110273605579</v>
+      </c>
+      <c r="R10">
+        <v>26</v>
+      </c>
+      <c r="S10">
+        <v>24</v>
+      </c>
+      <c r="T10">
+        <v>23</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B11">
+        <v>77163</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5.0955649029591932E-2</v>
+      </c>
+      <c r="D11">
+        <v>981492</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="5"/>
+        <v>0.44490424732304801</v>
+      </c>
+      <c r="F11">
+        <v>25.4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="6"/>
+        <v>0.41609195402298849</v>
+      </c>
+      <c r="H11">
+        <v>0.35398800000000002</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.37381724395951954</v>
+      </c>
+      <c r="J11">
+        <v>292764</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.65625601743353235</v>
+      </c>
+      <c r="L11">
+        <f>J11/D11</f>
+        <v>0.29828465234561258</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11" si="22">1-(L11/L$2)</f>
+        <v>0.38074831070358472</v>
+      </c>
+      <c r="N11">
+        <v>58279</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11" si="23">1-(N11/N$2)</f>
+        <v>0.14812974142341373</v>
+      </c>
+      <c r="P11">
+        <v>905312</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11" si="24">1-(P11/P$2)</f>
+        <v>0.46277481762891781</v>
+      </c>
+      <c r="R11">
+        <v>22</v>
+      </c>
+      <c r="S11">
+        <v>22</v>
+      </c>
+      <c r="T11">
+        <v>22</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>75718</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>6.8728015152633271E-2</v>
+      </c>
+      <c r="D13">
+        <v>525348</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="5"/>
+        <v>0.70288250594265533</v>
+      </c>
+      <c r="F13">
+        <v>13.9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="6"/>
+        <v>0.68045977011494252</v>
+      </c>
+      <c r="H13">
+        <v>1.603E-3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.99716439269711721</v>
+      </c>
+      <c r="J13">
+        <v>97138</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0.88594703249531515</v>
+      </c>
+      <c r="L13">
+        <f>J13/D13</f>
+        <v>0.18490219816198025</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13" si="25">1-(L13/L$2)</f>
+        <v>0.61613513244470153</v>
+      </c>
+      <c r="N13">
+        <v>44302</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13" si="26">1-(N13/N$2)</f>
+        <v>0.35243301711662989</v>
+      </c>
+      <c r="P13">
+        <v>316693</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13" si="27">1-(P13/P$2)</f>
+        <v>0.81206981164433345</v>
+      </c>
+      <c r="R13">
+        <v>20</v>
+      </c>
+      <c r="S13">
+        <v>20</v>
+      </c>
+      <c r="T13">
+        <v>19</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
+      <c r="B14">
+        <v>79227</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.5570068629621412E-2</v>
+      </c>
+      <c r="D14">
+        <v>967895</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
+        <v>0.452594210103334</v>
+      </c>
+      <c r="F14">
+        <v>24.4</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>0.43908045977011501</v>
+      </c>
+      <c r="H14">
+        <v>2.5140000000000002E-3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.99555289035592798</v>
+      </c>
+      <c r="J14">
+        <v>281050</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0.67000981575499119</v>
+      </c>
+      <c r="L14">
+        <f>J14/D14</f>
+        <v>0.29037240609776888</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14" si="28">1-(L14/L$2)</f>
+        <v>0.39717447214560664</v>
+      </c>
+      <c r="N14">
+        <v>60324</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14" si="29">1-(N14/N$2)</f>
+        <v>0.11823776182889212</v>
+      </c>
+      <c r="P14">
+        <v>778330</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ref="Q14" si="30">1-(P14/P$2)</f>
+        <v>0.53812776568201415</v>
+      </c>
+      <c r="R14">
+        <v>15</v>
+      </c>
+      <c r="S14">
+        <v>15</v>
+      </c>
+      <c r="T14">
+        <v>14</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>